<commit_message>
divide the original codes into two parts
</commit_message>
<xml_diff>
--- a/gis/silt/淤泥.xlsx
+++ b/gis/silt/淤泥.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:T35"/>
+  <dimension ref="A1:T58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -533,21 +533,21 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>243</v>
+        <v>68</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>CH2019GCZ20</t>
+          <t>CH201940ZK4</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>20.2</v>
+        <v>29.7</v>
       </c>
       <c r="D2" t="n">
-        <v>24.1</v>
+        <v>32.3</v>
       </c>
       <c r="E2" t="n">
-        <v>3.9</v>
+        <v>2.6</v>
       </c>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
@@ -560,63 +560,59 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>灰色</t>
+          <t>灰色，深灰色</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>灰色，软塑，黏性较好，干强度中等，中等韧性，切面稍有光泽</t>
+          <t>淤泥质土:灰色，深灰色，流塑，黏性较好，含有机质，具臭味，夹微薄层粉细砂。</t>
         </is>
       </c>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr">
         <is>
-          <t>软塑</t>
+          <t>流塑</t>
         </is>
       </c>
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="n">
-        <v>0.27</v>
+        <v>-0.52</v>
       </c>
       <c r="Q2" t="n">
-        <v>7237.87969050001</v>
+        <v>7029.03060600001</v>
       </c>
       <c r="R2" t="n">
-        <v>-4054.06297840116</v>
+        <v>2387.92326026534</v>
       </c>
       <c r="S2" t="n">
-        <v>-19.93</v>
+        <v>-30.22</v>
       </c>
       <c r="T2" t="n">
-        <v>-23.83</v>
+        <v>-32.82</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>421</v>
+        <v>243</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>CHGC001</t>
+          <t>CH2019GCZ20</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>21</v>
+        <v>20.2</v>
       </c>
       <c r="D3" t="n">
-        <v>21.6</v>
+        <v>24.1</v>
       </c>
       <c r="E3" t="n">
-        <v>0.600000000000001</v>
+        <v>3.9</v>
       </c>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>3-4</t>
-        </is>
-      </c>
+      <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr">
         <is>
           <t>淤泥质土</t>
@@ -624,54 +620,54 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>青灰色、浅灰色</t>
+          <t>灰色</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>深灰色，流-软塑，土质均一，具腥臭味</t>
+          <t>灰色，软塑，黏性较好，干强度中等，中等韧性，切面稍有光泽</t>
         </is>
       </c>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr">
         <is>
-          <t>流-软塑</t>
+          <t>软塑</t>
         </is>
       </c>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="n">
-        <v>2.27</v>
+        <v>0.27</v>
       </c>
       <c r="Q3" t="n">
-        <v>183.829200000007</v>
+        <v>7237.87969050001</v>
       </c>
       <c r="R3" t="n">
-        <v>458.441452265407</v>
+        <v>-4054.06297840116</v>
       </c>
       <c r="S3" t="n">
-        <v>-18.73</v>
+        <v>-19.93</v>
       </c>
       <c r="T3" t="n">
-        <v>-19.33</v>
+        <v>-23.83</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>456</v>
+        <v>369</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>CHGC002</t>
+          <t>CH2019GCZ33</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>26.35</v>
+        <v>29</v>
       </c>
       <c r="D4" t="n">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="E4" t="n">
-        <v>0.649999999999999</v>
+        <v>15</v>
       </c>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
@@ -679,72 +675,64 @@
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr">
         <is>
-          <t>淤泥质粉砂</t>
+          <t>淤泥质土</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>深灰色</t>
+          <t>灰色、深灰色</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>深灰色，饱和，松散状，成分为石英、云母，夹薄层粉砂</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>饱和</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>松散</t>
-        </is>
-      </c>
+          <t>灰色、深灰色，流塑，黏性较好，含有机质，具臭味，夹微薄层粉细砂</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>流塑</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr"/>
       <c r="P4" t="n">
-        <v>4.336</v>
+        <v>-3.6</v>
       </c>
       <c r="Q4" t="n">
-        <v>7326.61470000003</v>
+        <v>10244.2819455</v>
       </c>
       <c r="R4" t="n">
-        <v>-65.54454773447171</v>
+        <v>2977.90323226557</v>
       </c>
       <c r="S4" t="n">
-        <v>-22.014</v>
+        <v>-32.6</v>
       </c>
       <c r="T4" t="n">
-        <v>-22.664</v>
+        <v>-47.6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>479</v>
+        <v>385</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>CHGC003</t>
+          <t>CH2019GCZ35</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>18.1</v>
+        <v>26.5</v>
       </c>
       <c r="D5" t="n">
-        <v>19.9</v>
+        <v>36.2</v>
       </c>
       <c r="E5" t="n">
-        <v>1.8</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>3-4</t>
-        </is>
-      </c>
+      <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr">
         <is>
           <t>淤泥质土</t>
@@ -752,144 +740,136 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>深灰色</t>
+          <t>灰色、深灰色</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>深灰色，很湿，饱和，软塑状，成分为黏粉粒，稍含粉砂，见腐木</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>很湿-饱和</t>
-        </is>
-      </c>
+          <t>灰色、深灰色，流塑，黏性较好，含有机质，具臭味，夹微薄层粉细砂</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr">
         <is>
-          <t>软塑</t>
+          <t>流塑</t>
         </is>
       </c>
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="n">
-        <v>3.023</v>
+        <v>-4.29</v>
       </c>
       <c r="Q5" t="n">
-        <v>5682.28170000002</v>
+        <v>10707.4287885</v>
       </c>
       <c r="R5" t="n">
-        <v>-102.792547734454</v>
+        <v>1656.94619759886</v>
       </c>
       <c r="S5" t="n">
-        <v>-15.077</v>
+        <v>-30.79</v>
       </c>
       <c r="T5" t="n">
-        <v>-16.877</v>
+        <v>-40.49</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>492</v>
+        <v>421</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CHGC004</t>
+          <t>CHGC001</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>20.35</v>
+        <v>21</v>
       </c>
       <c r="D6" t="n">
-        <v>21.05</v>
+        <v>21.6</v>
       </c>
       <c r="E6" t="n">
-        <v>0.699999999999999</v>
+        <v>0.600000000000001</v>
       </c>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr">
         <is>
-          <t>2-4</t>
+          <t>3-4</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>含贝壳淤泥质土</t>
+          <t>淤泥质土</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>灰黑色</t>
+          <t>青灰色、浅灰色</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>灰黑色，流塑，土质不均，含大量贝壳碎片、味腥臭，含量约占65-70%</t>
+          <t>深灰色，流-软塑，土质均一，具腥臭味</t>
         </is>
       </c>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr">
         <is>
-          <t>流塑</t>
+          <t>流-软塑</t>
         </is>
       </c>
       <c r="O6" t="inlineStr"/>
       <c r="P6" t="n">
-        <v>3.634</v>
+        <v>2.27</v>
       </c>
       <c r="Q6" t="n">
-        <v>3098.7537</v>
+        <v>183.829200000007</v>
       </c>
       <c r="R6" t="n">
-        <v>-380.281214401126</v>
+        <v>458.441452265407</v>
       </c>
       <c r="S6" t="n">
-        <v>-16.716</v>
+        <v>-18.73</v>
       </c>
       <c r="T6" t="n">
-        <v>-17.416</v>
+        <v>-19.33</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>519</v>
+        <v>456</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>CHGC005</t>
+          <t>CHGC002</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>23.5</v>
+        <v>26.35</v>
       </c>
       <c r="D7" t="n">
-        <v>26.3</v>
+        <v>27</v>
       </c>
       <c r="E7" t="n">
-        <v>2.8</v>
+        <v>0.649999999999999</v>
       </c>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>2-4</t>
-        </is>
-      </c>
+      <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr">
         <is>
-          <t>含腐殖质淤泥质土</t>
+          <t>淤泥质粉砂</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>深灰色、灰黑色</t>
+          <t>深灰色</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>深灰色、灰黑色，饱和，流塑，土质不均匀，含少量腐殖质及有机质，味略腥臭</t>
+          <t>深灰色，饱和，松散状，成分为石英、云母，夹薄层粉砂</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -897,52 +877,52 @@
           <t>饱和</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>流塑</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>松散</t>
+        </is>
+      </c>
       <c r="P7" t="n">
-        <v>3.778</v>
+        <v>4.336</v>
       </c>
       <c r="Q7" t="n">
-        <v>2128.21620000005</v>
+        <v>7326.61470000003</v>
       </c>
       <c r="R7" t="n">
-        <v>385.064118932001</v>
+        <v>-65.54454773447171</v>
       </c>
       <c r="S7" t="n">
-        <v>-19.722</v>
+        <v>-22.014</v>
       </c>
       <c r="T7" t="n">
-        <v>-22.522</v>
+        <v>-22.664</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>551</v>
+        <v>479</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>CHGC007</t>
+          <t>CHGC003</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>22.2</v>
+        <v>18.1</v>
       </c>
       <c r="D8" t="n">
-        <v>25.6</v>
+        <v>19.9</v>
       </c>
       <c r="E8" t="n">
-        <v>3.4</v>
+        <v>1.8</v>
       </c>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr">
         <is>
-          <t>2-4</t>
+          <t>3-4</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -952,15 +932,19 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>深灰色、灰黑色</t>
+          <t>深灰色</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>深灰色、灰黑色，软塑，成份主要为粘粉粒，土质不均，其中22.20-24.00m含腐木及有机质，味腥臭，24.00-25.60m断续夹薄层中细砂或为泥砂互层。</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr"/>
+          <t>深灰色，很湿，饱和，软塑状，成分为黏粉粒，稍含粉砂，见腐木</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>很湿-饱和</t>
+        </is>
+      </c>
       <c r="N8" t="inlineStr">
         <is>
           <t>软塑</t>
@@ -968,38 +952,38 @@
       </c>
       <c r="O8" t="inlineStr"/>
       <c r="P8" t="n">
-        <v>2.064</v>
+        <v>3.023</v>
       </c>
       <c r="Q8" t="n">
-        <v>5417.1507</v>
+        <v>5682.28170000002</v>
       </c>
       <c r="R8" t="n">
-        <v>584.752118932083</v>
+        <v>-102.792547734454</v>
       </c>
       <c r="S8" t="n">
-        <v>-20.136</v>
+        <v>-15.077</v>
       </c>
       <c r="T8" t="n">
-        <v>-23.536</v>
+        <v>-16.877</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>572</v>
+        <v>492</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>CHGC008</t>
+          <t>CHGC004</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>19.3</v>
+        <v>20.35</v>
       </c>
       <c r="D9" t="n">
-        <v>29.8</v>
+        <v>21.05</v>
       </c>
       <c r="E9" t="n">
-        <v>10.5</v>
+        <v>0.699999999999999</v>
       </c>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
@@ -1011,81 +995,81 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>淤泥</t>
+          <t>含贝壳淤泥质土</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>深灰色、灰黑色</t>
+          <t>灰黑色</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>深灰色、灰黑色，软塑，具水平层理，土质均匀，切面滑腻，污手，粘性韧性较好，干强度中等。21.70-21.80m见不规则钙铁质结核团块，29.6-29.8为黑色，有机质含量高</t>
+          <t>灰黑色，流塑，土质不均，含大量贝壳碎片、味腥臭，含量约占65-70%</t>
         </is>
       </c>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr">
         <is>
-          <t>软塑</t>
+          <t>流塑</t>
         </is>
       </c>
       <c r="O9" t="inlineStr"/>
       <c r="P9" t="n">
-        <v>3.801</v>
+        <v>3.634</v>
       </c>
       <c r="Q9" t="n">
-        <v>6966.28920000003</v>
+        <v>3098.7537</v>
       </c>
       <c r="R9" t="n">
-        <v>638.735452265479</v>
+        <v>-380.281214401126</v>
       </c>
       <c r="S9" t="n">
-        <v>-15.499</v>
+        <v>-16.716</v>
       </c>
       <c r="T9" t="n">
-        <v>-25.999</v>
+        <v>-17.416</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>634</v>
+        <v>519</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>CHGC011</t>
+          <t>CHGC005</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>19.7</v>
+        <v>23.5</v>
       </c>
       <c r="D10" t="n">
-        <v>21.2</v>
+        <v>26.3</v>
       </c>
       <c r="E10" t="n">
-        <v>1.5</v>
+        <v>2.8</v>
       </c>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr">
         <is>
-          <t>3-1</t>
+          <t>2-4</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>淤泥质土</t>
+          <t>含腐殖质淤泥质土</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>深灰色</t>
+          <t>深灰色、灰黑色</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>深灰色，饱和，软塑，具腥臭味，主要由粘粉粒组成，土质不均匀，粉砂含量约占10-15%，20.70-20.90含腐木及腐殖质</t>
+          <t>深灰色、灰黑色，饱和，流塑，土质不均匀，含少量腐殖质及有机质，味略腥臭</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
@@ -1095,48 +1079,52 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>软塑</t>
+          <t>流塑</t>
         </is>
       </c>
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="n">
-        <v>1.615</v>
+        <v>3.778</v>
       </c>
       <c r="Q10" t="n">
-        <v>-139.644299999956</v>
+        <v>2128.21620000005</v>
       </c>
       <c r="R10" t="n">
-        <v>2981.97611893217</v>
+        <v>385.064118932001</v>
       </c>
       <c r="S10" t="n">
-        <v>-18.085</v>
+        <v>-19.722</v>
       </c>
       <c r="T10" t="n">
-        <v>-19.585</v>
+        <v>-22.522</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>637</v>
+        <v>551</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>CHGC011</t>
+          <t>CHGC007</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>23.2</v>
+        <v>22.2</v>
       </c>
       <c r="D11" t="n">
-        <v>29</v>
+        <v>25.6</v>
       </c>
       <c r="E11" t="n">
-        <v>5.8</v>
+        <v>3.4</v>
       </c>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>2-4</t>
+        </is>
+      </c>
       <c r="J11" t="inlineStr">
         <is>
           <t>淤泥质土</t>
@@ -1144,19 +1132,15 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>深灰色</t>
+          <t>深灰色、灰黑色</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>深灰色，饱和，软塑，具腥臭味。主要由粘粉粒组成，土质较均匀，28.30-28.50m为粉砂，略显水平层理</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>饱和</t>
-        </is>
-      </c>
+          <t>深灰色、灰黑色，软塑，成份主要为粘粉粒，土质不均，其中22.20-24.00m含腐木及有机质，味腥臭，24.00-25.60m断续夹薄层中细砂或为泥砂互层。</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr">
         <is>
           <t>软塑</t>
@@ -1164,128 +1148,124 @@
       </c>
       <c r="O11" t="inlineStr"/>
       <c r="P11" t="n">
-        <v>1.615</v>
+        <v>2.064</v>
       </c>
       <c r="Q11" t="n">
-        <v>-139.644299999956</v>
+        <v>5417.1507</v>
       </c>
       <c r="R11" t="n">
-        <v>2981.97611893217</v>
+        <v>584.752118932083</v>
       </c>
       <c r="S11" t="n">
-        <v>-21.585</v>
+        <v>-20.136</v>
       </c>
       <c r="T11" t="n">
-        <v>-27.385</v>
+        <v>-23.536</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>721</v>
+        <v>572</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>CHGC015</t>
+          <t>CHGC008</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>20.7</v>
+        <v>19.3</v>
       </c>
       <c r="D12" t="n">
-        <v>26</v>
+        <v>29.8</v>
       </c>
       <c r="E12" t="n">
-        <v>5.3</v>
+        <v>10.5</v>
       </c>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>2-4</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>含粉砂淤泥质土</t>
+          <t>淤泥</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>深灰色</t>
+          <t>深灰色、灰黑色</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>深灰色，饱和、流塑成分主要为黏粒，土质不均，断续夹薄层砂或为泥砂互层水平层理</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>饱和</t>
-        </is>
-      </c>
+          <t>深灰色、灰黑色，软塑，具水平层理，土质均匀，切面滑腻，污手，粘性韧性较好，干强度中等。21.70-21.80m见不规则钙铁质结核团块，29.6-29.8为黑色，有机质含量高</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr">
         <is>
-          <t>流塑</t>
+          <t>软塑</t>
         </is>
       </c>
       <c r="O12" t="inlineStr"/>
       <c r="P12" t="n">
-        <v>1.738</v>
+        <v>3.801</v>
       </c>
       <c r="Q12" t="n">
-        <v>4666.26120000001</v>
+        <v>6966.28920000003</v>
       </c>
       <c r="R12" t="n">
-        <v>2633.77878559877</v>
+        <v>638.735452265479</v>
       </c>
       <c r="S12" t="n">
-        <v>-18.962</v>
+        <v>-15.499</v>
       </c>
       <c r="T12" t="n">
-        <v>-24.262</v>
+        <v>-25.999</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>722</v>
+        <v>634</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>CHGC015</t>
+          <t>CHGC011</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>26</v>
+        <v>19.7</v>
       </c>
       <c r="D13" t="n">
-        <v>30.5</v>
+        <v>21.2</v>
       </c>
       <c r="E13" t="n">
-        <v>4.5</v>
+        <v>1.5</v>
       </c>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>3-1</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>淤泥</t>
+          <t>淤泥质土</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>深灰色、灰黑色</t>
+          <t>深灰色</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>深灰色、灰黑色、饱和，流塑、质均、滑腻、沾手，粘性韧性良好、干强度较高，水平层理</t>
+          <t>深灰色，饱和，软塑，具腥臭味，主要由粘粉粒组成，土质不均匀，粉砂含量约占10-15%，20.70-20.90含腐木及腐殖质</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
@@ -1295,55 +1275,51 @@
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>流塑</t>
+          <t>软塑</t>
         </is>
       </c>
       <c r="O13" t="inlineStr"/>
       <c r="P13" t="n">
-        <v>1.738</v>
+        <v>1.615</v>
       </c>
       <c r="Q13" t="n">
-        <v>4666.26120000001</v>
+        <v>-139.644299999956</v>
       </c>
       <c r="R13" t="n">
-        <v>2633.77878559877</v>
+        <v>2981.97611893217</v>
       </c>
       <c r="S13" t="n">
-        <v>-24.262</v>
+        <v>-18.085</v>
       </c>
       <c r="T13" t="n">
-        <v>-28.762</v>
+        <v>-19.585</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>723</v>
+        <v>637</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>CHGC015</t>
+          <t>CHGC011</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>30.5</v>
+        <v>23.2</v>
       </c>
       <c r="D14" t="n">
-        <v>31.2</v>
+        <v>29</v>
       </c>
       <c r="E14" t="n">
-        <v>0.699999999999999</v>
+        <v>5.8</v>
       </c>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
-      <c r="I14" t="inlineStr">
-        <is>
-          <t>3-4</t>
-        </is>
-      </c>
+      <c r="I14" t="inlineStr"/>
       <c r="J14" t="inlineStr">
         <is>
-          <t>含腐木淤泥质土</t>
+          <t>淤泥质土</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
@@ -1353,7 +1329,7 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>深灰色、饱和，流塑、具腐臭味主要由粉粒组成，腐木含量约占10-15%</t>
+          <t>深灰色，饱和，软塑，具腥臭味。主要由粘粉粒组成，土质较均匀，28.30-28.50m为粉砂，略显水平层理</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
@@ -1363,133 +1339,125 @@
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>流塑</t>
+          <t>软塑</t>
         </is>
       </c>
       <c r="O14" t="inlineStr"/>
       <c r="P14" t="n">
-        <v>1.738</v>
+        <v>1.615</v>
       </c>
       <c r="Q14" t="n">
-        <v>4666.26120000001</v>
+        <v>-139.644299999956</v>
       </c>
       <c r="R14" t="n">
-        <v>2633.77878559877</v>
+        <v>2981.97611893217</v>
       </c>
       <c r="S14" t="n">
-        <v>-28.762</v>
+        <v>-21.585</v>
       </c>
       <c r="T14" t="n">
-        <v>-29.462</v>
+        <v>-27.385</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>937</v>
+        <v>671</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>CHGC025</t>
+          <t>CHGC013</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>23.3</v>
+        <v>33.2</v>
       </c>
       <c r="D15" t="n">
-        <v>24.3</v>
+        <v>33.85</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>0.649999999999999</v>
       </c>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
-      <c r="I15" t="inlineStr">
-        <is>
-          <t>2-4</t>
-        </is>
-      </c>
+      <c r="I15" t="inlineStr"/>
       <c r="J15" t="inlineStr">
         <is>
-          <t>含淤泥粉砂</t>
+          <t>淤泥质土</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>深灰色，灰黑色</t>
+          <t>深灰色</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>深灰色，灰黑色，饱和，稍密状，砂粒成份为石英，含较多淤泥黏粒，分选性较好，级配较差</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>饱和</t>
-        </is>
-      </c>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>稍密</t>
-        </is>
-      </c>
+          <t>深灰色，软塑，主要成份为粘粒，含有机质，具腐臭味，干强度高，韧性中等.33.20-33.30m为浅灰色，33.70mm见腐殖质</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>软塑</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr"/>
       <c r="P15" t="n">
-        <v>4.153</v>
+        <v>3.389</v>
       </c>
       <c r="Q15" t="n">
-        <v>6420.39720000001</v>
+        <v>1848.01770000005</v>
       </c>
       <c r="R15" t="n">
-        <v>3856.97678559863</v>
+        <v>2464.18278559887</v>
       </c>
       <c r="S15" t="n">
-        <v>-19.147</v>
+        <v>-29.811</v>
       </c>
       <c r="T15" t="n">
-        <v>-20.147</v>
+        <v>-30.461</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>938</v>
+        <v>721</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>CHGC025</t>
+          <t>CHGC015</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>24.3</v>
+        <v>20.7</v>
       </c>
       <c r="D16" t="n">
-        <v>27.6</v>
+        <v>26</v>
       </c>
       <c r="E16" t="n">
-        <v>3.3</v>
+        <v>5.3</v>
       </c>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
       <c r="I16" t="inlineStr">
         <is>
-          <t>2-4</t>
+          <t>3-4</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>含粉砂淤泥</t>
+          <t>含粉砂淤泥质土</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>深灰色，灰黑色</t>
+          <t>深灰色</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>深灰色，灰黑色，饱和，软塑状，成份为黏、粉粒，含有机质，局部夹薄层粉砂，25.0-25.1m为含淤泥粉砂</t>
+          <t>深灰色，饱和、流塑成分主要为黏粒，土质不均，断续夹薄层砂或为泥砂互层水平层理</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
@@ -1499,183 +1467,179 @@
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>软塑</t>
+          <t>流塑</t>
         </is>
       </c>
       <c r="O16" t="inlineStr"/>
       <c r="P16" t="n">
-        <v>4.153</v>
+        <v>1.738</v>
       </c>
       <c r="Q16" t="n">
-        <v>6420.39720000001</v>
+        <v>4666.26120000001</v>
       </c>
       <c r="R16" t="n">
-        <v>3856.97678559863</v>
+        <v>2633.77878559877</v>
       </c>
       <c r="S16" t="n">
-        <v>-20.147</v>
+        <v>-18.962</v>
       </c>
       <c r="T16" t="n">
-        <v>-23.447</v>
+        <v>-24.262</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>939</v>
+        <v>722</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>CHGC025</t>
+          <t>CHGC015</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>27.6</v>
+        <v>26</v>
       </c>
       <c r="D17" t="n">
-        <v>30</v>
+        <v>30.5</v>
       </c>
       <c r="E17" t="n">
-        <v>2.4</v>
+        <v>4.5</v>
       </c>
       <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
       <c r="I17" t="inlineStr">
         <is>
-          <t>2-4</t>
+          <t>3-4</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>含腐木淤泥质土</t>
+          <t>淤泥</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>深灰色，灰黑色</t>
+          <t>深灰色、灰黑色</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>深灰色，灰黑色，很湿～饱和，软塑状，成份为黏、粉粒，含腐木，29.2～29.6m含较多粉细砂，水平层理</t>
+          <t>深灰色、灰黑色、饱和，流塑、质均、滑腻、沾手，粘性韧性良好、干强度较高，水平层理</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>很湿-饱和</t>
+          <t>饱和</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>软塑</t>
+          <t>流塑</t>
         </is>
       </c>
       <c r="O17" t="inlineStr"/>
       <c r="P17" t="n">
-        <v>4.153</v>
+        <v>1.738</v>
       </c>
       <c r="Q17" t="n">
-        <v>6420.39720000001</v>
+        <v>4666.26120000001</v>
       </c>
       <c r="R17" t="n">
-        <v>3856.97678559863</v>
+        <v>2633.77878559877</v>
       </c>
       <c r="S17" t="n">
-        <v>-23.447</v>
+        <v>-24.262</v>
       </c>
       <c r="T17" t="n">
-        <v>-25.847</v>
+        <v>-28.762</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>940</v>
+        <v>723</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>CHGC025</t>
+          <t>CHGC015</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>30</v>
+        <v>30.5</v>
       </c>
       <c r="D18" t="n">
-        <v>32.3</v>
+        <v>31.2</v>
       </c>
       <c r="E18" t="n">
-        <v>2.3</v>
+        <v>0.699999999999999</v>
       </c>
       <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
       <c r="I18" t="inlineStr">
         <is>
-          <t>2-4</t>
+          <t>3-4</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>淤泥质土</t>
+          <t>含腐木淤泥质土</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>深灰色，灰黑色</t>
+          <t>深灰色</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>深灰色，灰黑色，很湿～饱和，软塑状，成份为黏、粉粒，含有机质，散体结构</t>
+          <t>深灰色、饱和，流塑、具腐臭味主要由粉粒组成，腐木含量约占10-15%</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>很湿-饱和</t>
+          <t>饱和</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>软塑</t>
-        </is>
-      </c>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>散体结构</t>
-        </is>
-      </c>
+          <t>流塑</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr"/>
       <c r="P18" t="n">
-        <v>4.153</v>
+        <v>1.738</v>
       </c>
       <c r="Q18" t="n">
-        <v>6420.39720000001</v>
+        <v>4666.26120000001</v>
       </c>
       <c r="R18" t="n">
-        <v>3856.97678559863</v>
+        <v>2633.77878559877</v>
       </c>
       <c r="S18" t="n">
-        <v>-25.847</v>
+        <v>-28.762</v>
       </c>
       <c r="T18" t="n">
-        <v>-28.147</v>
+        <v>-29.462</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>967</v>
+        <v>725</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>CHGC026</t>
+          <t>CHGC015</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>30.3</v>
+        <v>31.7</v>
       </c>
       <c r="D19" t="n">
-        <v>33.1</v>
+        <v>32</v>
       </c>
       <c r="E19" t="n">
-        <v>2.8</v>
+        <v>0.300000000000001</v>
       </c>
       <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
@@ -1683,17 +1647,17 @@
       <c r="I19" t="inlineStr"/>
       <c r="J19" t="inlineStr">
         <is>
-          <t>含粉砂淤泥质土</t>
+          <t>含腐木淤泥质土</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>深灰色、灰黑色</t>
+          <t>深灰色</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>深灰色、灰黑色，饱和，软塑状，成份为黏、粉粒，含有机质，具腥臭味，水平层理，30.5～30.7m为粉砂夹层，局部为粉砂与淤泥质土互层</t>
+          <t>深灰色、饱和，流塑、具腥臭味，土质不均，腐木含量约占10-15%</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
@@ -1703,65 +1667,61 @@
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>软塑</t>
+          <t>流塑</t>
         </is>
       </c>
       <c r="O19" t="inlineStr"/>
       <c r="P19" t="n">
-        <v>3.536</v>
+        <v>1.738</v>
       </c>
       <c r="Q19" t="n">
-        <v>5722.62570000003</v>
+        <v>4666.26120000001</v>
       </c>
       <c r="R19" t="n">
-        <v>4466.66211893223</v>
+        <v>2633.77878559877</v>
       </c>
       <c r="S19" t="n">
-        <v>-26.764</v>
+        <v>-29.962</v>
       </c>
       <c r="T19" t="n">
-        <v>-29.564</v>
+        <v>-30.262</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>989</v>
+        <v>729</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>CHGC027</t>
+          <t>CHGC015</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>19.1</v>
+        <v>37.8</v>
       </c>
       <c r="D20" t="n">
-        <v>28.8</v>
+        <v>39.6</v>
       </c>
       <c r="E20" t="n">
-        <v>9.699999999999999</v>
+        <v>1.8</v>
       </c>
       <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
-      <c r="I20" t="inlineStr">
-        <is>
-          <t>2-4</t>
-        </is>
-      </c>
+      <c r="I20" t="inlineStr"/>
       <c r="J20" t="inlineStr">
         <is>
-          <t>淤泥质土</t>
+          <t>含粉砂淤泥质土</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>深灰色，灰黑色</t>
+          <t>深灰色</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>深灰色，灰黑色，饱和，流塑-软塑，成分以粘粉粒为主，含有机质。19.4-19.5含贝壳碎屑。28.5-28.6m含贝壳碎屑及蚝壳，28.6-28.8m含植物腐殖质</t>
+          <t>深灰色，饱和、软塑具腥臭味，主要由粉粒组成，夹薄层粉砂，粉砂含量约占5%</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
@@ -1771,65 +1731,61 @@
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>流塑</t>
+          <t>软塑</t>
         </is>
       </c>
       <c r="O20" t="inlineStr"/>
       <c r="P20" t="n">
-        <v>3.959</v>
+        <v>1.738</v>
       </c>
       <c r="Q20" t="n">
-        <v>4750.63920000006</v>
+        <v>4666.26120000001</v>
       </c>
       <c r="R20" t="n">
-        <v>4916.19211893218</v>
+        <v>2633.77878559877</v>
       </c>
       <c r="S20" t="n">
-        <v>-15.141</v>
+        <v>-36.062</v>
       </c>
       <c r="T20" t="n">
-        <v>-24.841</v>
+        <v>-37.862</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>1042</v>
+        <v>910</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>CHGC029</t>
+          <t>CHGC024</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>27</v>
+        <v>39.6</v>
       </c>
       <c r="D21" t="n">
-        <v>30</v>
+        <v>40.7</v>
       </c>
       <c r="E21" t="n">
-        <v>3</v>
+        <v>1.1</v>
       </c>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr">
-        <is>
-          <t>3-4</t>
-        </is>
-      </c>
+      <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr">
         <is>
-          <t>淤泥质土</t>
+          <t>含粉砂淤泥质土</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>深灰色，灰黑色</t>
+          <t>灰-深灰夹浅灰条纹</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>深灰色，灰黑色，饱和，软塑状，成分为黏粉粒，夹薄层粉砂</t>
+          <t>灰-深灰夹浅灰条纹，粉砂厚度约1-3mm，主要含细粒砂就粗粉砂，均一性较好，淤泥质土层约4-6mm，主要由粉黏粒组成，含少量有机质。具砂泥水平互层层理，饱和，软塑～流塑状</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
@@ -1844,106 +1800,106 @@
       </c>
       <c r="O21" t="inlineStr"/>
       <c r="P21" t="n">
-        <v>3.781</v>
+        <v>3.26</v>
       </c>
       <c r="Q21" t="n">
-        <v>3489.26670000001</v>
+        <v>5332.17120000001</v>
       </c>
       <c r="R21" t="n">
-        <v>5070.16945226553</v>
+        <v>3887.00078559884</v>
       </c>
       <c r="S21" t="n">
-        <v>-23.219</v>
+        <v>-36.34</v>
       </c>
       <c r="T21" t="n">
-        <v>-26.219</v>
+        <v>-37.44</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>1044</v>
+        <v>937</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>CHGC029</t>
+          <t>CHGC025</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>30.3</v>
+        <v>23.3</v>
       </c>
       <c r="D22" t="n">
-        <v>30.8</v>
+        <v>24.3</v>
       </c>
       <c r="E22" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr"/>
       <c r="I22" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>2-4</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>淤泥质土</t>
+          <t>含淤泥粉砂</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>深灰色</t>
+          <t>深灰色，灰黑色</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>深灰色，很湿，软塑，成分为黏、粉粒，夹薄层粉砂</t>
+          <t>深灰色，灰黑色，饱和，稍密状，砂粒成份为石英，含较多淤泥黏粒，分选性较好，级配较差</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>很湿</t>
-        </is>
-      </c>
-      <c r="N22" t="inlineStr">
-        <is>
-          <t>软塑</t>
-        </is>
-      </c>
-      <c r="O22" t="inlineStr"/>
+          <t>饱和</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>稍密</t>
+        </is>
+      </c>
       <c r="P22" t="n">
-        <v>3.781</v>
+        <v>4.153</v>
       </c>
       <c r="Q22" t="n">
-        <v>3489.26670000001</v>
+        <v>6420.39720000001</v>
       </c>
       <c r="R22" t="n">
-        <v>5070.16945226553</v>
+        <v>3856.97678559863</v>
       </c>
       <c r="S22" t="n">
-        <v>-26.519</v>
+        <v>-19.147</v>
       </c>
       <c r="T22" t="n">
-        <v>-27.019</v>
+        <v>-20.147</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>1073</v>
+        <v>938</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>CHGC030</t>
+          <t>CHGC025</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>18.45</v>
+        <v>24.3</v>
       </c>
       <c r="D23" t="n">
-        <v>24.7</v>
+        <v>27.6</v>
       </c>
       <c r="E23" t="n">
-        <v>6.25</v>
+        <v>3.3</v>
       </c>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr"/>
@@ -1955,22 +1911,22 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>淤泥质土夹粉砂薄层</t>
+          <t>含粉砂淤泥</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>深灰色</t>
+          <t>深灰色，灰黑色</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>深灰色，很湿，软塑，主要成分为粘粉粒，含有机质，不均匀夹2-5mm粉砂薄层，具腐臭味，局部含少量贝壳碎屑</t>
+          <t>深灰色，灰黑色，饱和，软塑状，成份为黏、粉粒，含有机质，局部夹薄层粉砂，25.0-25.1m为含淤泥粉砂</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>很湿</t>
+          <t>饱和</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
@@ -1980,38 +1936,38 @@
       </c>
       <c r="O23" t="inlineStr"/>
       <c r="P23" t="n">
-        <v>3.238</v>
+        <v>4.153</v>
       </c>
       <c r="Q23" t="n">
-        <v>3398.29920000007</v>
+        <v>6420.39720000001</v>
       </c>
       <c r="R23" t="n">
-        <v>5448.07678559888</v>
+        <v>3856.97678559863</v>
       </c>
       <c r="S23" t="n">
-        <v>-15.212</v>
+        <v>-20.147</v>
       </c>
       <c r="T23" t="n">
-        <v>-21.462</v>
+        <v>-23.447</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>1074</v>
+        <v>939</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>CHGC030</t>
+          <t>CHGC025</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>24.7</v>
+        <v>27.6</v>
       </c>
       <c r="D24" t="n">
         <v>30</v>
       </c>
       <c r="E24" t="n">
-        <v>5.3</v>
+        <v>2.4</v>
       </c>
       <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr"/>
@@ -2023,22 +1979,22 @@
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>淤泥质土</t>
+          <t>含腐木淤泥质土</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>深灰色、灰黑色</t>
+          <t>深灰色，灰黑色</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>深灰色、灰黑色，很湿，软塑，主要成分为粘粒，含有机质及腐殖质，局部偶含少量贝壳碎屑，干强度及韧性高。其中27.70m-27.80m为腐木，28.67m-30.00m含腐殖质较多</t>
+          <t>深灰色，灰黑色，很湿～饱和，软塑状，成份为黏、粉粒，含腐木，29.2～29.6m含较多粉细砂，水平层理</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>很湿</t>
+          <t>很湿-饱和</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
@@ -2048,38 +2004,38 @@
       </c>
       <c r="O24" t="inlineStr"/>
       <c r="P24" t="n">
-        <v>3.238</v>
+        <v>4.153</v>
       </c>
       <c r="Q24" t="n">
-        <v>3398.29920000007</v>
+        <v>6420.39720000001</v>
       </c>
       <c r="R24" t="n">
-        <v>5448.07678559888</v>
+        <v>3856.97678559863</v>
       </c>
       <c r="S24" t="n">
-        <v>-21.462</v>
+        <v>-23.447</v>
       </c>
       <c r="T24" t="n">
-        <v>-26.762</v>
+        <v>-25.847</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>1442</v>
+        <v>940</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>CHS002</t>
+          <t>CHGC025</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D25" t="n">
-        <v>25</v>
+        <v>32.3</v>
       </c>
       <c r="E25" t="n">
-        <v>3</v>
+        <v>2.3</v>
       </c>
       <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr"/>
@@ -2091,85 +2047,85 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>含粉砂质淤泥质土</t>
+          <t>淤泥质土</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>深灰色</t>
+          <t>深灰色，灰黑色</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>含粉砂质淤泥质土：深灰色，饱和，流塑，具腥臭味，主要由粘粉粒组成。粉砂含量约20--30%，局部夹贝壳碎屑。</t>
+          <t>深灰色，灰黑色，很湿～饱和，软塑状，成份为黏、粉粒，含有机质，散体结构</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>饱和</t>
+          <t>很湿-饱和</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>流塑</t>
-        </is>
-      </c>
-      <c r="O25" t="inlineStr"/>
+          <t>软塑</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>散体结构</t>
+        </is>
+      </c>
       <c r="P25" t="n">
-        <v>6.797</v>
+        <v>4.153</v>
       </c>
       <c r="Q25" t="n">
-        <v>1593.23220000003</v>
+        <v>6420.39720000001</v>
       </c>
       <c r="R25" t="n">
-        <v>5589.67611893204</v>
+        <v>3856.97678559863</v>
       </c>
       <c r="S25" t="n">
-        <v>-15.203</v>
+        <v>-25.847</v>
       </c>
       <c r="T25" t="n">
-        <v>-18.203</v>
+        <v>-28.147</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>1444</v>
+        <v>967</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>CHS002</t>
+          <t>CHGC026</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>28.9</v>
+        <v>30.3</v>
       </c>
       <c r="D26" t="n">
-        <v>33.99</v>
+        <v>33.1</v>
       </c>
       <c r="E26" t="n">
-        <v>5.09</v>
+        <v>2.8</v>
       </c>
       <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr"/>
       <c r="H26" t="inlineStr"/>
-      <c r="I26" t="inlineStr">
-        <is>
-          <t>2-4</t>
-        </is>
-      </c>
+      <c r="I26" t="inlineStr"/>
       <c r="J26" t="inlineStr">
         <is>
-          <t>淤泥质土</t>
+          <t>含粉砂淤泥质土</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>深灰色</t>
+          <t>深灰色、灰黑色</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>淤泥质土：深灰色，饱和，流塑，具腥臭味，主要由粘粉粒组成，土质较均匀，切面较光滑。</t>
+          <t>深灰色、灰黑色，饱和，软塑状，成份为黏、粉粒，含有机质，具腥臭味，水平层理，30.5～30.7m为粉砂夹层，局部为粉砂与淤泥质土互层</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
@@ -2179,65 +2135,65 @@
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>流塑</t>
+          <t>软塑</t>
         </is>
       </c>
       <c r="O26" t="inlineStr"/>
       <c r="P26" t="n">
-        <v>6.797</v>
+        <v>3.536</v>
       </c>
       <c r="Q26" t="n">
-        <v>1593.23220000003</v>
+        <v>5722.62570000003</v>
       </c>
       <c r="R26" t="n">
-        <v>5589.67611893204</v>
+        <v>4466.66211893223</v>
       </c>
       <c r="S26" t="n">
-        <v>-22.103</v>
+        <v>-26.764</v>
       </c>
       <c r="T26" t="n">
-        <v>-27.193</v>
+        <v>-29.564</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>1514</v>
+        <v>989</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>CHS018</t>
+          <t>CHGC027</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>22</v>
+        <v>19.1</v>
       </c>
       <c r="D27" t="n">
-        <v>26.8</v>
+        <v>28.8</v>
       </c>
       <c r="E27" t="n">
-        <v>4.8</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr"/>
       <c r="H27" t="inlineStr"/>
       <c r="I27" t="inlineStr">
         <is>
-          <t>3-4</t>
+          <t>2-4</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>粉砂质淤泥</t>
+          <t>淤泥质土</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>深灰</t>
+          <t>深灰色，灰黑色</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>深灰；饱和；软塑；含较多粉砂。</t>
+          <t>深灰色，灰黑色，饱和，流塑-软塑，成分以粘粉粒为主，含有机质。19.4-19.5含贝壳碎屑。28.5-28.6m含贝壳碎屑及蚝壳，28.6-28.8m含植物腐殖质</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
@@ -2247,43 +2203,43 @@
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>软塑</t>
+          <t>流塑</t>
         </is>
       </c>
       <c r="O27" t="inlineStr"/>
       <c r="P27" t="n">
-        <v>4</v>
+        <v>3.959</v>
       </c>
       <c r="Q27" t="n">
-        <v>2931.17970000007</v>
+        <v>4750.63920000006</v>
       </c>
       <c r="R27" t="n">
-        <v>4928.08011893214</v>
+        <v>4916.19211893218</v>
       </c>
       <c r="S27" t="n">
-        <v>-18</v>
+        <v>-15.141</v>
       </c>
       <c r="T27" t="n">
-        <v>-22.8</v>
+        <v>-24.841</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>1536</v>
+        <v>1020</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>CHS021</t>
+          <t>CHGC028</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>25</v>
+        <v>32.4</v>
       </c>
       <c r="D28" t="n">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>3.6</v>
       </c>
       <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr"/>
@@ -2295,17 +2251,17 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>淤泥质土</t>
+          <t>含粉砂淤泥质土</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>灰~深灰色</t>
+          <t>深灰色、灰黑色</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>淤泥质土：灰~深灰色，饱和，流塑；主要为粘粒，含少量腐殖质及有机质，具腐臭味。</t>
+          <t>深灰色、灰黑色，饱和，软塑状，成份为黏、粉粒，含有机质，局部夹薄层粉砂，水平层理</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
@@ -2315,70 +2271,65 @@
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>流塑</t>
+          <t>软塑</t>
         </is>
       </c>
       <c r="O28" t="inlineStr"/>
       <c r="P28" t="n">
-        <v>3.06</v>
+        <v>2.706</v>
       </c>
       <c r="Q28" t="n">
-        <v>3515.67870000002</v>
+        <v>4588.13370000006</v>
       </c>
       <c r="R28" t="n">
-        <v>4558.90745226542</v>
+        <v>4583.84345226549</v>
       </c>
       <c r="S28" t="n">
-        <v>-21.94</v>
+        <v>-29.694</v>
       </c>
       <c r="T28" t="n">
-        <v>-22.94</v>
+        <v>-33.294</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>1580</v>
+        <v>1042</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>CHS027</t>
+          <t>CHGC029</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>13.65</v>
+        <v>27</v>
       </c>
       <c r="D29" t="n">
-        <v>25.95</v>
+        <v>30</v>
       </c>
       <c r="E29" t="n">
-        <v>12.3</v>
+        <v>3</v>
       </c>
       <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr"/>
-      <c r="H29" t="inlineStr">
-        <is>
-          <t>Qhhl</t>
-        </is>
-      </c>
+      <c r="H29" t="inlineStr"/>
       <c r="I29" t="inlineStr">
         <is>
-          <t>2-4</t>
+          <t>3-4</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>淤泥</t>
+          <t>淤泥质土</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>灰色</t>
+          <t>深灰色，灰黑色</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t xml:space="preserve">淤泥:灰色，饱和，流塑，含云母及腐植物，局部夹薄层砂，略具异味。
-</t>
+          <t>深灰色，灰黑色，饱和，软塑状，成分为黏粉粒，夹薄层粉砂</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
@@ -2388,139 +2339,134 @@
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>流塑</t>
+          <t>软塑</t>
         </is>
       </c>
       <c r="O29" t="inlineStr"/>
       <c r="P29" t="n">
-        <v>-2.116</v>
+        <v>3.781</v>
       </c>
       <c r="Q29" t="n">
-        <v>9170.41893449999</v>
+        <v>3489.26670000001</v>
       </c>
       <c r="R29" t="n">
-        <v>3738.9778229321</v>
+        <v>5070.16945226553</v>
       </c>
       <c r="S29" t="n">
-        <v>-15.766</v>
+        <v>-23.219</v>
       </c>
       <c r="T29" t="n">
-        <v>-28.066</v>
+        <v>-26.219</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>1597</v>
+        <v>1044</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>CHS035</t>
+          <t>CHGC029</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>24.8</v>
+        <v>30.3</v>
       </c>
       <c r="D30" t="n">
-        <v>25.7</v>
+        <v>30.8</v>
       </c>
       <c r="E30" t="n">
-        <v>0.899999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr"/>
-      <c r="I30" t="inlineStr"/>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>3-4</t>
+        </is>
+      </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>淤泥质粉质黏土</t>
+          <t>淤泥质土</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>灰色-灰黄色</t>
+          <t>深灰色</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t xml:space="preserve">淤泥质粉质黏土:灰色-灰黄色，饱和，流塑，间夹粉细砂，分布不均。
-</t>
+          <t>深灰色，很湿，软塑，成分为黏、粉粒，夹薄层粉砂</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>饱和</t>
+          <t>很湿</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>流塑</t>
+          <t>软塑</t>
         </is>
       </c>
       <c r="O30" t="inlineStr"/>
       <c r="P30" t="n">
-        <v>-2.896</v>
+        <v>3.781</v>
       </c>
       <c r="Q30" t="n">
-        <v>7015.87897649998</v>
+        <v>3489.26670000001</v>
       </c>
       <c r="R30" t="n">
-        <v>3479.78898826552</v>
+        <v>5070.16945226553</v>
       </c>
       <c r="S30" t="n">
-        <v>-27.696</v>
+        <v>-26.519</v>
       </c>
       <c r="T30" t="n">
-        <v>-28.596</v>
+        <v>-27.019</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>1642</v>
+        <v>1046</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>CHS056</t>
+          <t>CHGC029</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>20.1</v>
+        <v>33.2</v>
       </c>
       <c r="D31" t="n">
-        <v>23.2</v>
+        <v>34.3</v>
       </c>
       <c r="E31" t="n">
-        <v>3.1</v>
+        <v>1.09999999999999</v>
       </c>
       <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr"/>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>Qpx</t>
-        </is>
-      </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>3-4</t>
-        </is>
-      </c>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr"/>
       <c r="J31" t="inlineStr">
         <is>
-          <t>淤泥质粉质粘土</t>
+          <t>含粉砂淤泥质土</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>深灰色</t>
+          <t>深灰色，灰黑色</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>淤泥质粉质粘土:深灰色,饱和,软塑,含少量有机质及贝壳碎屑,局部夹粉细砂簿层,易污手,具腥臭味。</t>
+          <t>深灰色，灰黑色，很湿，软塑，成分为黏、粉粒，夹薄层或不规则团状粉砂</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>饱和</t>
+          <t>很湿</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
@@ -2530,38 +2476,38 @@
       </c>
       <c r="O31" t="inlineStr"/>
       <c r="P31" t="n">
-        <v>3.45</v>
+        <v>3.781</v>
       </c>
       <c r="Q31" t="n">
-        <v>-1811.43329999998</v>
+        <v>3489.26670000001</v>
       </c>
       <c r="R31" t="n">
-        <v>2352.68811893215</v>
+        <v>5070.16945226553</v>
       </c>
       <c r="S31" t="n">
-        <v>-16.65</v>
+        <v>-29.419</v>
       </c>
       <c r="T31" t="n">
-        <v>-19.75</v>
+        <v>-30.519</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>1667</v>
+        <v>1073</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>CHS072</t>
+          <t>CHGC030</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>20</v>
+        <v>18.45</v>
       </c>
       <c r="D32" t="n">
-        <v>26.6</v>
+        <v>24.7</v>
       </c>
       <c r="E32" t="n">
-        <v>6.6</v>
+        <v>6.25</v>
       </c>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr"/>
@@ -2573,7 +2519,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>含腐木淤泥质土</t>
+          <t>淤泥质土夹粉砂薄层</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2583,10 +2529,14 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>含腐木淤泥质土：深灰色夹褐色，软塑，主要为粘粉粒，含腐木及有机质，具腐臭味。</t>
-        </is>
-      </c>
-      <c r="M32" t="inlineStr"/>
+          <t>深灰色，很湿，软塑，主要成分为粘粉粒，含有机质，不均匀夹2-5mm粉砂薄层，具腐臭味，局部含少量贝壳碎屑</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>很湿</t>
+        </is>
+      </c>
       <c r="N32" t="inlineStr">
         <is>
           <t>软塑</t>
@@ -2594,59 +2544,67 @@
       </c>
       <c r="O32" t="inlineStr"/>
       <c r="P32" t="n">
-        <v>4.59</v>
+        <v>3.238</v>
       </c>
       <c r="Q32" t="n">
-        <v>4528.43369999999</v>
+        <v>3398.29920000007</v>
       </c>
       <c r="R32" t="n">
-        <v>3275.40211893215</v>
+        <v>5448.07678559888</v>
       </c>
       <c r="S32" t="n">
-        <v>-15.41</v>
+        <v>-15.212</v>
       </c>
       <c r="T32" t="n">
-        <v>-22.01</v>
+        <v>-21.462</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>1669</v>
+        <v>1074</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>CHS072</t>
+          <t>CHGC030</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>29</v>
+        <v>24.7</v>
       </c>
       <c r="D33" t="n">
-        <v>29.8</v>
+        <v>30</v>
       </c>
       <c r="E33" t="n">
-        <v>0.800000000000001</v>
+        <v>5.3</v>
       </c>
       <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr"/>
       <c r="H33" t="inlineStr"/>
-      <c r="I33" t="inlineStr"/>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>2-4</t>
+        </is>
+      </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>含粉砂淤泥质土</t>
+          <t>淤泥质土</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>深灰色</t>
+          <t>深灰色、灰黑色</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>含粉砂淤泥质土：深灰色，软塑；主要为粘粉粒，含有机质，局部夹薄层粉砂，具腐臭味。</t>
-        </is>
-      </c>
-      <c r="M33" t="inlineStr"/>
+          <t>深灰色、灰黑色，很湿，软塑，主要成分为粘粒，含有机质及腐殖质，局部偶含少量贝壳碎屑，干强度及韧性高。其中27.70m-27.80m为腐木，28.67m-30.00m含腐殖质较多</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>很湿</t>
+        </is>
+      </c>
       <c r="N33" t="inlineStr">
         <is>
           <t>软塑</t>
@@ -2654,98 +2612,94 @@
       </c>
       <c r="O33" t="inlineStr"/>
       <c r="P33" t="n">
-        <v>4.59</v>
+        <v>3.238</v>
       </c>
       <c r="Q33" t="n">
-        <v>4528.43369999999</v>
+        <v>3398.29920000007</v>
       </c>
       <c r="R33" t="n">
-        <v>3275.40211893215</v>
+        <v>5448.07678559888</v>
       </c>
       <c r="S33" t="n">
-        <v>-24.41</v>
+        <v>-21.462</v>
       </c>
       <c r="T33" t="n">
-        <v>-25.21</v>
+        <v>-26.762</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>1671</v>
+        <v>1418</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>CHS072</t>
+          <t>CHS001</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>31</v>
+        <v>34.5</v>
       </c>
       <c r="D34" t="n">
-        <v>31.9</v>
+        <v>47.25</v>
       </c>
       <c r="E34" t="n">
-        <v>0.899999999999999</v>
+        <v>12.75</v>
       </c>
       <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr"/>
       <c r="H34" t="inlineStr"/>
-      <c r="I34" t="inlineStr"/>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>2-4</t>
+        </is>
+      </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>含粉砂淤泥质土</t>
-        </is>
-      </c>
-      <c r="K34" t="inlineStr">
-        <is>
-          <t>深灰色</t>
-        </is>
-      </c>
+          <t>淤泥质中细砂与淤泥质粘土</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr"/>
       <c r="L34" t="inlineStr">
         <is>
-          <t>含粉砂淤泥质土：深灰色，软塑；主要为粘粉粒，含有机质，局部夹薄层粉砂，具腐臭味。</t>
+          <t>淤泥质中细砂与淤泥质粘土：二者相间分布比例不均，3:1-1:2之间变化。该层以淤泥质中细砂为主，且其内见大量小贝壳发育，粒度明显较上层变粗。往下部淤泥质中细砂含量有增加、变粗趋势。</t>
         </is>
       </c>
       <c r="M34" t="inlineStr"/>
-      <c r="N34" t="inlineStr">
-        <is>
-          <t>软塑</t>
-        </is>
-      </c>
+      <c r="N34" t="inlineStr"/>
       <c r="O34" t="inlineStr"/>
       <c r="P34" t="n">
-        <v>4.59</v>
+        <v>4.576</v>
       </c>
       <c r="Q34" t="n">
-        <v>4528.43369999999</v>
+        <v>5692.32570000002</v>
       </c>
       <c r="R34" t="n">
-        <v>3275.40211893215</v>
+        <v>6535.87278559866</v>
       </c>
       <c r="S34" t="n">
-        <v>-26.41</v>
+        <v>-29.924</v>
       </c>
       <c r="T34" t="n">
-        <v>-27.31</v>
+        <v>-42.674</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>2063</v>
+        <v>1420</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>HJS004</t>
+          <t>CHS001</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>22.5</v>
+        <v>53</v>
       </c>
       <c r="D35" t="n">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="E35" t="n">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr"/>
@@ -2753,44 +2707,1563 @@
       <c r="I35" t="inlineStr"/>
       <c r="J35" t="inlineStr">
         <is>
+          <t>淤泥质细砂夹淤泥质粘土</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr"/>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>淤泥质细砂夹淤泥质粘土：二者比例5:1-4：1之间变化。淤泥质细砂，砂感明显，湿，饱和。淤泥质粘土，湿，软塑。与上层相比颜色变化，为深灰、灰黑色，应形成于还原环境。</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>湿饱和</t>
+        </is>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>软塑</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr"/>
+      <c r="P35" t="n">
+        <v>4.576</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>5692.32570000002</v>
+      </c>
+      <c r="R35" t="n">
+        <v>6535.87278559866</v>
+      </c>
+      <c r="S35" t="n">
+        <v>-48.424</v>
+      </c>
+      <c r="T35" t="n">
+        <v>-49.424</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>1442</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>CHS002</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>22</v>
+      </c>
+      <c r="D36" t="n">
+        <v>25</v>
+      </c>
+      <c r="E36" t="n">
+        <v>3</v>
+      </c>
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="inlineStr"/>
+      <c r="H36" t="inlineStr"/>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>2-4</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>含粉砂质淤泥质土</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>深灰色</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>含粉砂质淤泥质土：深灰色，饱和，流塑，具腥臭味，主要由粘粉粒组成。粉砂含量约20--30%，局部夹贝壳碎屑。</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>饱和</t>
+        </is>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>流塑</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr"/>
+      <c r="P36" t="n">
+        <v>6.797</v>
+      </c>
+      <c r="Q36" t="n">
+        <v>1593.23220000003</v>
+      </c>
+      <c r="R36" t="n">
+        <v>5589.67611893204</v>
+      </c>
+      <c r="S36" t="n">
+        <v>-15.203</v>
+      </c>
+      <c r="T36" t="n">
+        <v>-18.203</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>1444</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>CHS002</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>28.9</v>
+      </c>
+      <c r="D37" t="n">
+        <v>33.99</v>
+      </c>
+      <c r="E37" t="n">
+        <v>5.09</v>
+      </c>
+      <c r="F37" t="inlineStr"/>
+      <c r="G37" t="inlineStr"/>
+      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>2-4</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>淤泥质土</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>深灰色</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>淤泥质土：深灰色，饱和，流塑，具腥臭味，主要由粘粉粒组成，土质较均匀，切面较光滑。</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>饱和</t>
+        </is>
+      </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>流塑</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr"/>
+      <c r="P37" t="n">
+        <v>6.797</v>
+      </c>
+      <c r="Q37" t="n">
+        <v>1593.23220000003</v>
+      </c>
+      <c r="R37" t="n">
+        <v>5589.67611893204</v>
+      </c>
+      <c r="S37" t="n">
+        <v>-22.103</v>
+      </c>
+      <c r="T37" t="n">
+        <v>-27.193</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>1488</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>CHS004</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>43</v>
+      </c>
+      <c r="D38" t="n">
+        <v>44.5</v>
+      </c>
+      <c r="E38" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr"/>
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>3-4</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>淤泥质土</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>深灰色</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>淤泥质土：深灰色，饱和，流塑，具腥臭味，主要由粘粉粒组成，局部含腐木。</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>饱和</t>
+        </is>
+      </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>流塑</t>
+        </is>
+      </c>
+      <c r="O38" t="inlineStr"/>
+      <c r="P38" t="n">
+        <v>3.458</v>
+      </c>
+      <c r="Q38" t="n">
+        <v>-2449.40879999995</v>
+      </c>
+      <c r="R38" t="n">
+        <v>5338.31478559878</v>
+      </c>
+      <c r="S38" t="n">
+        <v>-39.542</v>
+      </c>
+      <c r="T38" t="n">
+        <v>-41.042</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>1489</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>CHS004</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>44.5</v>
+      </c>
+      <c r="D39" t="n">
+        <v>46</v>
+      </c>
+      <c r="E39" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="inlineStr"/>
+      <c r="H39" t="inlineStr"/>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>3-4</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>含腐木质淤泥质土</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>深灰色</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>含腐木质淤泥质土：深灰色，饱和，流塑，具腥臭味，主要由粘粉粒组成，腐木含量约占10%~20%。</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>饱和</t>
+        </is>
+      </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>流塑</t>
+        </is>
+      </c>
+      <c r="O39" t="inlineStr"/>
+      <c r="P39" t="n">
+        <v>3.458</v>
+      </c>
+      <c r="Q39" t="n">
+        <v>-2449.40879999995</v>
+      </c>
+      <c r="R39" t="n">
+        <v>5338.31478559878</v>
+      </c>
+      <c r="S39" t="n">
+        <v>-41.042</v>
+      </c>
+      <c r="T39" t="n">
+        <v>-42.542</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>1490</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>CHS004</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>46</v>
+      </c>
+      <c r="D40" t="n">
+        <v>46.5</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr"/>
+      <c r="H40" t="inlineStr"/>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>3-4</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>淤泥质土</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>深灰色</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>淤泥质土：深灰色，饱和，流塑，具腥臭味，主要由粘粉粒组成，局部含腐木。</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>饱和</t>
+        </is>
+      </c>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>流塑</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr"/>
+      <c r="P40" t="n">
+        <v>3.458</v>
+      </c>
+      <c r="Q40" t="n">
+        <v>-2449.40879999995</v>
+      </c>
+      <c r="R40" t="n">
+        <v>5338.31478559878</v>
+      </c>
+      <c r="S40" t="n">
+        <v>-42.542</v>
+      </c>
+      <c r="T40" t="n">
+        <v>-43.042</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>1514</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>CHS018</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>22</v>
+      </c>
+      <c r="D41" t="n">
+        <v>26.8</v>
+      </c>
+      <c r="E41" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="inlineStr"/>
+      <c r="H41" t="inlineStr"/>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>3-4</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>粉砂质淤泥</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>深灰</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>深灰；饱和；软塑；含较多粉砂。</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>饱和</t>
+        </is>
+      </c>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>软塑</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr"/>
+      <c r="P41" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q41" t="n">
+        <v>2931.17970000007</v>
+      </c>
+      <c r="R41" t="n">
+        <v>4928.08011893214</v>
+      </c>
+      <c r="S41" t="n">
+        <v>-18</v>
+      </c>
+      <c r="T41" t="n">
+        <v>-22.8</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>1515</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>CHS018</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>26.8</v>
+      </c>
+      <c r="D42" t="n">
+        <v>34.5</v>
+      </c>
+      <c r="E42" t="n">
+        <v>7.7</v>
+      </c>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="inlineStr"/>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>3-4</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>淤泥</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>深灰色</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>深灰色；湿；可塑；呈粘土状；已固结。</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>湿</t>
+        </is>
+      </c>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>可塑</t>
+        </is>
+      </c>
+      <c r="O42" t="inlineStr"/>
+      <c r="P42" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q42" t="n">
+        <v>2931.17970000007</v>
+      </c>
+      <c r="R42" t="n">
+        <v>4928.08011893214</v>
+      </c>
+      <c r="S42" t="n">
+        <v>-22.8</v>
+      </c>
+      <c r="T42" t="n">
+        <v>-30.5</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>1516</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>CHS018</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>34.5</v>
+      </c>
+      <c r="D43" t="n">
+        <v>36</v>
+      </c>
+      <c r="E43" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F43" t="inlineStr"/>
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="inlineStr"/>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>3-4</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>粉砂质淤泥</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>深灰</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>深灰；饱和；软塑；中部含较多腐殖质。</t>
+        </is>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>饱和</t>
+        </is>
+      </c>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>软塑</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr"/>
+      <c r="P43" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q43" t="n">
+        <v>2931.17970000007</v>
+      </c>
+      <c r="R43" t="n">
+        <v>4928.08011893214</v>
+      </c>
+      <c r="S43" t="n">
+        <v>-30.5</v>
+      </c>
+      <c r="T43" t="n">
+        <v>-32</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>1517</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>CHS018</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>36</v>
+      </c>
+      <c r="D44" t="n">
+        <v>38</v>
+      </c>
+      <c r="E44" t="n">
+        <v>2</v>
+      </c>
+      <c r="F44" t="inlineStr"/>
+      <c r="G44" t="inlineStr"/>
+      <c r="H44" t="inlineStr"/>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>3-4</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>淤泥</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>灰黑</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>灰黑；很湿；可塑；含多量腐木；已碳化；呈半固结状态。</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>很湿</t>
+        </is>
+      </c>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>可塑</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr"/>
+      <c r="P44" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q44" t="n">
+        <v>2931.17970000007</v>
+      </c>
+      <c r="R44" t="n">
+        <v>4928.08011893214</v>
+      </c>
+      <c r="S44" t="n">
+        <v>-32</v>
+      </c>
+      <c r="T44" t="n">
+        <v>-34</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>1536</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>CHS021</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>25</v>
+      </c>
+      <c r="D45" t="n">
+        <v>26</v>
+      </c>
+      <c r="E45" t="n">
+        <v>1</v>
+      </c>
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="inlineStr"/>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>3-4</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>淤泥质土</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>灰~深灰色</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>淤泥质土：灰~深灰色，饱和，流塑；主要为粘粒，含少量腐殖质及有机质，具腐臭味。</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>饱和</t>
+        </is>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>流塑</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr"/>
+      <c r="P45" t="n">
+        <v>3.06</v>
+      </c>
+      <c r="Q45" t="n">
+        <v>3515.67870000002</v>
+      </c>
+      <c r="R45" t="n">
+        <v>4558.90745226542</v>
+      </c>
+      <c r="S45" t="n">
+        <v>-21.94</v>
+      </c>
+      <c r="T45" t="n">
+        <v>-22.94</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>1540</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>CHS021</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>30.2</v>
+      </c>
+      <c r="D46" t="n">
+        <v>34.5</v>
+      </c>
+      <c r="E46" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="F46" t="inlineStr"/>
+      <c r="G46" t="inlineStr"/>
+      <c r="H46" t="inlineStr"/>
+      <c r="I46" t="inlineStr"/>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>淤泥质土</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>深灰色</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>淤泥质土：深灰色，灰黑色，饱和，流塑；含少量石英砂及腐木碎屑。</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>饱和</t>
+        </is>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>流塑</t>
+        </is>
+      </c>
+      <c r="O46" t="inlineStr"/>
+      <c r="P46" t="n">
+        <v>3.06</v>
+      </c>
+      <c r="Q46" t="n">
+        <v>3515.67870000002</v>
+      </c>
+      <c r="R46" t="n">
+        <v>4558.90745226542</v>
+      </c>
+      <c r="S46" t="n">
+        <v>-27.14</v>
+      </c>
+      <c r="T46" t="n">
+        <v>-31.44</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>1542</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>CHS021</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>37.4</v>
+      </c>
+      <c r="D47" t="n">
+        <v>41.1</v>
+      </c>
+      <c r="E47" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="F47" t="inlineStr"/>
+      <c r="G47" t="inlineStr"/>
+      <c r="H47" t="inlineStr"/>
+      <c r="I47" t="inlineStr"/>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>淤泥质土</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>深灰色</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>淤泥质土：深灰色，软塑；含有机质及少量腐木碎屑，土质较均匀。</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr"/>
+      <c r="N47" t="inlineStr">
+        <is>
+          <t>软塑</t>
+        </is>
+      </c>
+      <c r="O47" t="inlineStr"/>
+      <c r="P47" t="n">
+        <v>3.06</v>
+      </c>
+      <c r="Q47" t="n">
+        <v>3515.67870000002</v>
+      </c>
+      <c r="R47" t="n">
+        <v>4558.90745226542</v>
+      </c>
+      <c r="S47" t="n">
+        <v>-34.34</v>
+      </c>
+      <c r="T47" t="n">
+        <v>-38.04</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>1580</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>CHS027</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>13.65</v>
+      </c>
+      <c r="D48" t="n">
+        <v>25.95</v>
+      </c>
+      <c r="E48" t="n">
+        <v>12.3</v>
+      </c>
+      <c r="F48" t="inlineStr"/>
+      <c r="G48" t="inlineStr"/>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>Qhhl</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>2-4</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>淤泥</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>灰色</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">淤泥:灰色，饱和，流塑，含云母及腐植物，局部夹薄层砂，略具异味。
+</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>饱和</t>
+        </is>
+      </c>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>流塑</t>
+        </is>
+      </c>
+      <c r="O48" t="inlineStr"/>
+      <c r="P48" t="n">
+        <v>-2.116</v>
+      </c>
+      <c r="Q48" t="n">
+        <v>9170.41893449999</v>
+      </c>
+      <c r="R48" t="n">
+        <v>3738.9778229321</v>
+      </c>
+      <c r="S48" t="n">
+        <v>-15.766</v>
+      </c>
+      <c r="T48" t="n">
+        <v>-28.066</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>1581</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>CHS027</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>25.95</v>
+      </c>
+      <c r="D49" t="n">
+        <v>30.7</v>
+      </c>
+      <c r="E49" t="n">
+        <v>4.75</v>
+      </c>
+      <c r="F49" t="inlineStr"/>
+      <c r="G49" t="inlineStr"/>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>Qhhl</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>2-4</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>淤泥质黏土</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>灰色</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">淤泥质黏土:灰色，饱和，流塑，含贝屑及少许腐植物，局部夹薄层砂。
+</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>饱和</t>
+        </is>
+      </c>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>流塑</t>
+        </is>
+      </c>
+      <c r="O49" t="inlineStr"/>
+      <c r="P49" t="n">
+        <v>-2.116</v>
+      </c>
+      <c r="Q49" t="n">
+        <v>9170.41893449999</v>
+      </c>
+      <c r="R49" t="n">
+        <v>3738.9778229321</v>
+      </c>
+      <c r="S49" t="n">
+        <v>-28.066</v>
+      </c>
+      <c r="T49" t="n">
+        <v>-32.816</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>1597</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>CHS035</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>24.8</v>
+      </c>
+      <c r="D50" t="n">
+        <v>25.7</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.899999999999999</v>
+      </c>
+      <c r="F50" t="inlineStr"/>
+      <c r="G50" t="inlineStr"/>
+      <c r="H50" t="inlineStr"/>
+      <c r="I50" t="inlineStr"/>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>淤泥质粉质黏土</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>灰色-灰黄色</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t xml:space="preserve">淤泥质粉质黏土:灰色-灰黄色，饱和，流塑，间夹粉细砂，分布不均。
+</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>饱和</t>
+        </is>
+      </c>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>流塑</t>
+        </is>
+      </c>
+      <c r="O50" t="inlineStr"/>
+      <c r="P50" t="n">
+        <v>-2.896</v>
+      </c>
+      <c r="Q50" t="n">
+        <v>7015.87897649998</v>
+      </c>
+      <c r="R50" t="n">
+        <v>3479.78898826552</v>
+      </c>
+      <c r="S50" t="n">
+        <v>-27.696</v>
+      </c>
+      <c r="T50" t="n">
+        <v>-28.596</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>1642</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>CHS056</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>20.1</v>
+      </c>
+      <c r="D51" t="n">
+        <v>23.2</v>
+      </c>
+      <c r="E51" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="F51" t="inlineStr"/>
+      <c r="G51" t="inlineStr"/>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>Qpx</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>3-4</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>淤泥质粉质粘土</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>深灰色</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>淤泥质粉质粘土:深灰色,饱和,软塑,含少量有机质及贝壳碎屑,局部夹粉细砂簿层,易污手,具腥臭味。</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>饱和</t>
+        </is>
+      </c>
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>软塑</t>
+        </is>
+      </c>
+      <c r="O51" t="inlineStr"/>
+      <c r="P51" t="n">
+        <v>3.45</v>
+      </c>
+      <c r="Q51" t="n">
+        <v>-1811.43329999998</v>
+      </c>
+      <c r="R51" t="n">
+        <v>2352.68811893215</v>
+      </c>
+      <c r="S51" t="n">
+        <v>-16.65</v>
+      </c>
+      <c r="T51" t="n">
+        <v>-19.75</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>1667</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>CHS072</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>20</v>
+      </c>
+      <c r="D52" t="n">
+        <v>26.6</v>
+      </c>
+      <c r="E52" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="F52" t="inlineStr"/>
+      <c r="G52" t="inlineStr"/>
+      <c r="H52" t="inlineStr"/>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>2-4</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>含腐木淤泥质土</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>深灰色</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>含腐木淤泥质土：深灰色夹褐色，软塑，主要为粘粉粒，含腐木及有机质，具腐臭味。</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr"/>
+      <c r="N52" t="inlineStr">
+        <is>
+          <t>软塑</t>
+        </is>
+      </c>
+      <c r="O52" t="inlineStr"/>
+      <c r="P52" t="n">
+        <v>4.59</v>
+      </c>
+      <c r="Q52" t="n">
+        <v>4528.43369999999</v>
+      </c>
+      <c r="R52" t="n">
+        <v>3275.40211893215</v>
+      </c>
+      <c r="S52" t="n">
+        <v>-15.41</v>
+      </c>
+      <c r="T52" t="n">
+        <v>-22.01</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>1669</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>CHS072</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>29</v>
+      </c>
+      <c r="D53" t="n">
+        <v>29.8</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0.800000000000001</v>
+      </c>
+      <c r="F53" t="inlineStr"/>
+      <c r="G53" t="inlineStr"/>
+      <c r="H53" t="inlineStr"/>
+      <c r="I53" t="inlineStr"/>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>含粉砂淤泥质土</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>深灰色</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>含粉砂淤泥质土：深灰色，软塑；主要为粘粉粒，含有机质，局部夹薄层粉砂，具腐臭味。</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr"/>
+      <c r="N53" t="inlineStr">
+        <is>
+          <t>软塑</t>
+        </is>
+      </c>
+      <c r="O53" t="inlineStr"/>
+      <c r="P53" t="n">
+        <v>4.59</v>
+      </c>
+      <c r="Q53" t="n">
+        <v>4528.43369999999</v>
+      </c>
+      <c r="R53" t="n">
+        <v>3275.40211893215</v>
+      </c>
+      <c r="S53" t="n">
+        <v>-24.41</v>
+      </c>
+      <c r="T53" t="n">
+        <v>-25.21</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>1671</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>CHS072</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>31</v>
+      </c>
+      <c r="D54" t="n">
+        <v>31.9</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0.899999999999999</v>
+      </c>
+      <c r="F54" t="inlineStr"/>
+      <c r="G54" t="inlineStr"/>
+      <c r="H54" t="inlineStr"/>
+      <c r="I54" t="inlineStr"/>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>含粉砂淤泥质土</t>
+        </is>
+      </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>深灰色</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>含粉砂淤泥质土：深灰色，软塑；主要为粘粉粒，含有机质，局部夹薄层粉砂，具腐臭味。</t>
+        </is>
+      </c>
+      <c r="M54" t="inlineStr"/>
+      <c r="N54" t="inlineStr">
+        <is>
+          <t>软塑</t>
+        </is>
+      </c>
+      <c r="O54" t="inlineStr"/>
+      <c r="P54" t="n">
+        <v>4.59</v>
+      </c>
+      <c r="Q54" t="n">
+        <v>4528.43369999999</v>
+      </c>
+      <c r="R54" t="n">
+        <v>3275.40211893215</v>
+      </c>
+      <c r="S54" t="n">
+        <v>-26.41</v>
+      </c>
+      <c r="T54" t="n">
+        <v>-27.31</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>1991</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>CHSW01</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>30.2</v>
+      </c>
+      <c r="D55" t="n">
+        <v>33.6</v>
+      </c>
+      <c r="E55" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="F55" t="inlineStr"/>
+      <c r="G55" t="inlineStr"/>
+      <c r="H55" t="inlineStr"/>
+      <c r="I55" t="inlineStr"/>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>淤泥质粘土</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>深灰-灰黑色</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>深灰-灰黑色，主要由粉砂、有机质及粘粒组成，粉砂含量约5-10%，粉砂与粘土互层，粉砂厚度1-2.5cm不等，贝壳碎屑含量较少，约5%；局部见灰色泥质结核，粒径0.5-1.5cm；闻有腥臭味，可塑，该段为隔水层，弱透水性。</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr"/>
+      <c r="N55" t="inlineStr">
+        <is>
+          <t>可塑</t>
+        </is>
+      </c>
+      <c r="O55" t="inlineStr"/>
+      <c r="P55" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="Q55" t="n">
+        <v>3732.8052</v>
+      </c>
+      <c r="R55" t="n">
+        <v>4788.45078559872</v>
+      </c>
+      <c r="S55" t="n">
+        <v>-26.7</v>
+      </c>
+      <c r="T55" t="n">
+        <v>-30.1</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>2063</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>HJS004</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="D56" t="n">
+        <v>24</v>
+      </c>
+      <c r="E56" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="F56" t="inlineStr"/>
+      <c r="G56" t="inlineStr"/>
+      <c r="H56" t="inlineStr"/>
+      <c r="I56" t="inlineStr"/>
+      <c r="J56" t="inlineStr">
+        <is>
           <t>淤泥质中细砂</t>
         </is>
       </c>
-      <c r="K35" t="inlineStr">
+      <c r="K56" t="inlineStr">
         <is>
           <t>深灰色</t>
         </is>
       </c>
-      <c r="L35" t="inlineStr">
+      <c r="L56" t="inlineStr">
         <is>
           <t>深灰色淤泥质中细砂，砂含量约为70%，由上至下，砂的直径逐渐变大，砂中包含有石英颗粒 ，砾径小于2mm，淤泥质含量约为25%,其他可见少量砾石，大小约为2-3mm，整体结构松散，密实度差，含水率高，饱水。</t>
         </is>
       </c>
-      <c r="M35" t="inlineStr">
+      <c r="M56" t="inlineStr">
         <is>
           <t>饱水</t>
         </is>
       </c>
-      <c r="N35" t="inlineStr"/>
-      <c r="O35" t="inlineStr">
+      <c r="N56" t="inlineStr"/>
+      <c r="O56" t="inlineStr">
         <is>
           <t>松散</t>
         </is>
       </c>
-      <c r="P35" t="n">
+      <c r="P56" t="n">
         <v>2</v>
       </c>
-      <c r="Q35" t="n">
+      <c r="Q56" t="n">
         <v>-17063.5923</v>
       </c>
-      <c r="R35" t="n">
+      <c r="R56" t="n">
         <v>832.394785598852</v>
       </c>
-      <c r="S35" t="n">
+      <c r="S56" t="n">
         <v>-20.5</v>
       </c>
-      <c r="T35" t="n">
+      <c r="T56" t="n">
         <v>-22</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>2110</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>MZS002</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>23.9</v>
+      </c>
+      <c r="D57" t="n">
+        <v>41.55</v>
+      </c>
+      <c r="E57" t="n">
+        <v>17.65</v>
+      </c>
+      <c r="F57" t="inlineStr"/>
+      <c r="G57" t="inlineStr"/>
+      <c r="H57" t="inlineStr"/>
+      <c r="I57" t="inlineStr"/>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>淤泥质土</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>深灰色</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>淤泥质土:深灰色，饱和，软塑状为主。切面光滑，干强度一般，局部含少量粉细砂，韧性低。</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>饱和</t>
+        </is>
+      </c>
+      <c r="N57" t="inlineStr">
+        <is>
+          <t>软塑</t>
+        </is>
+      </c>
+      <c r="O57" t="inlineStr"/>
+      <c r="P57" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q57" t="n">
+        <v>-3847.13279999993</v>
+      </c>
+      <c r="R57" t="n">
+        <v>5664.91611893227</v>
+      </c>
+      <c r="S57" t="n">
+        <v>-22.9</v>
+      </c>
+      <c r="T57" t="n">
+        <v>-40.55</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>2111</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>MZS002</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>41.55</v>
+      </c>
+      <c r="D58" t="n">
+        <v>46.34</v>
+      </c>
+      <c r="E58" t="n">
+        <v>4.79</v>
+      </c>
+      <c r="F58" t="inlineStr"/>
+      <c r="G58" t="inlineStr"/>
+      <c r="H58" t="inlineStr"/>
+      <c r="I58" t="inlineStr"/>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>淤泥质粉细砂</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>深灰色</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>淤泥质粉细砂:深灰色，饱和，松散。混含40%淤泥，中下部淤泥质含量减少。</t>
+        </is>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>饱和</t>
+        </is>
+      </c>
+      <c r="N58" t="inlineStr"/>
+      <c r="O58" t="inlineStr">
+        <is>
+          <t>松散</t>
+        </is>
+      </c>
+      <c r="P58" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q58" t="n">
+        <v>-3847.13279999993</v>
+      </c>
+      <c r="R58" t="n">
+        <v>5664.91611893227</v>
+      </c>
+      <c r="S58" t="n">
+        <v>-40.55</v>
+      </c>
+      <c r="T58" t="n">
+        <v>-45.34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>